<commit_message>
Converted the units to the needed ones
</commit_message>
<xml_diff>
--- a/output/input_for_scenario_analysis.xlsx
+++ b/output/input_for_scenario_analysis.xlsx
@@ -559,14 +559,14 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K2" t="n">
         <v>2015</v>
       </c>
       <c r="L2" t="n">
-        <v>2.567784294916357e-05</v>
+        <v>92.44023461698886</v>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
@@ -577,7 +577,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -630,14 +630,14 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K3" t="n">
         <v>2015</v>
       </c>
       <c r="L3" t="n">
-        <v>8.052778745701137e-06</v>
+        <v>28.9900034845241</v>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -648,7 +648,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -719,7 +719,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -772,14 +772,14 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1000m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K5" t="n">
         <v>2015</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0205748851717017</v>
+        <v>20.5748851717017</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
@@ -790,7 +790,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -861,7 +861,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -914,7 +914,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1056,14 +1056,14 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>km / capita</t>
+          <t>tkm/cap/year</t>
         </is>
       </c>
       <c r="K9" t="n">
         <v>2015</v>
       </c>
       <c r="L9" t="n">
-        <v>1.059754755692944e-05</v>
+        <v>10597.54755692944</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="K10" t="n">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal/cap/year</t>
         </is>
       </c>
       <c r="K11" t="n">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1269,14 +1269,14 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K12" t="n">
         <v>2015</v>
       </c>
       <c r="L12" t="n">
-        <v>4.091521796827101e-07</v>
+        <v>0.4091521796827101</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -1340,14 +1340,14 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K13" t="n">
         <v>2015</v>
       </c>
       <c r="L13" t="n">
-        <v>5.255786268492357e-07</v>
+        <v>0.5255786268492357</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -1411,14 +1411,14 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K14" t="n">
         <v>2050</v>
       </c>
       <c r="L14" t="n">
-        <v>1.13950786213136e-05</v>
+        <v>41.02228303672896</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -1482,14 +1482,14 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K15" t="n">
         <v>2050</v>
       </c>
       <c r="L15" t="n">
-        <v>3.860456692526717e-06</v>
+        <v>13.89764409309618</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K16" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -1624,14 +1624,14 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1000m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K17" t="n">
         <v>2050</v>
       </c>
       <c r="L17" t="n">
-        <v>0.02021879437211879</v>
+        <v>20.21879437211879</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K18" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K19" t="n">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K20" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -1908,14 +1908,14 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>km / capita</t>
+          <t>tkm/cap/year</t>
         </is>
       </c>
       <c r="K21" t="n">
         <v>2050</v>
       </c>
       <c r="L21" t="n">
-        <v>8.123025418079452e-06</v>
+        <v>8123.025418079452</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="K22" t="n">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal/cap/year</t>
         </is>
       </c>
       <c r="K23" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -2121,14 +2121,14 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K24" t="n">
         <v>2050</v>
       </c>
       <c r="L24" t="n">
-        <v>2.050796055697152e-07</v>
+        <v>0.2050796055697152</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
@@ -2192,14 +2192,14 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K25" t="n">
         <v>2050</v>
       </c>
       <c r="L25" t="n">
-        <v>3.14260784468168e-07</v>
+        <v>0.314260784468168</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
@@ -2263,14 +2263,14 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K26" t="n">
         <v>2015</v>
       </c>
       <c r="L26" t="n">
-        <v>2.065623758877241e-05</v>
+        <v>74.36245531958068</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
@@ -2334,14 +2334,14 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K27" t="n">
         <v>2015</v>
       </c>
       <c r="L27" t="n">
-        <v>5.756364339753717e-06</v>
+        <v>20.72291162311338</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K28" t="n">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
@@ -2476,14 +2476,14 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1000m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K29" t="n">
         <v>2015</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01469473041515453</v>
+        <v>14.69473041515453</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K30" t="n">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K31" t="n">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
@@ -2689,7 +2689,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K32" t="n">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
@@ -2760,14 +2760,14 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>km / capita</t>
+          <t>tkm/cap/year</t>
         </is>
       </c>
       <c r="K33" t="n">
         <v>2015</v>
       </c>
       <c r="L33" t="n">
-        <v>7.217520129121297e-06</v>
+        <v>7217.520129121297</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
@@ -2778,7 +2778,7 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="K34" t="n">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal/cap/year</t>
         </is>
       </c>
       <c r="K35" t="n">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
@@ -2973,14 +2973,14 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K36" t="n">
         <v>2015</v>
       </c>
       <c r="L36" t="n">
-        <v>3.423666033624484e-07</v>
+        <v>0.3423666033624484</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
@@ -3044,14 +3044,14 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K37" t="n">
         <v>2015</v>
       </c>
       <c r="L37" t="n">
-        <v>3.21444484124084e-07</v>
+        <v>0.321444484124084</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
@@ -3115,14 +3115,14 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K38" t="n">
         <v>2050</v>
       </c>
       <c r="L38" t="n">
-        <v>1.021644698640537e-05</v>
+        <v>36.77920915105934</v>
       </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
@@ -3186,14 +3186,14 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>TWh / capita</t>
+          <t>GJ/cap/year</t>
         </is>
       </c>
       <c r="K39" t="n">
         <v>2050</v>
       </c>
       <c r="L39" t="n">
-        <v>3.581020983349488e-06</v>
+        <v>12.89167554005816</v>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
@@ -3257,7 +3257,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K40" t="n">
@@ -3275,7 +3275,7 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
@@ -3328,14 +3328,14 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>1000m2 / capita</t>
+          <t>m²/cap</t>
         </is>
       </c>
       <c r="K41" t="n">
         <v>2050</v>
       </c>
       <c r="L41" t="n">
-        <v>0.01412437952123616</v>
+        <v>14.12437952123616</v>
       </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K42" t="n">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
@@ -3470,7 +3470,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K43" t="n">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>pkm / capita</t>
+          <t>pkm/cap/year</t>
         </is>
       </c>
       <c r="K44" t="n">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
@@ -3612,14 +3612,14 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>km / capita</t>
+          <t>tkm/cap/year</t>
         </is>
       </c>
       <c r="K45" t="n">
         <v>2050</v>
       </c>
       <c r="L45" t="n">
-        <v>5.411159829960237e-06</v>
+        <v>5411.159829960237</v>
       </c>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
@@ -3630,7 +3630,7 @@
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
@@ -3683,7 +3683,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal meat/cap/day</t>
         </is>
       </c>
       <c r="K46" t="n">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>kcal / capita</t>
+          <t>kcal/cap/year</t>
         </is>
       </c>
       <c r="K47" t="n">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
@@ -3825,14 +3825,14 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K48" t="n">
         <v>2050</v>
       </c>
       <c r="L48" t="n">
-        <v>1.856341912613852e-07</v>
+        <v>0.1856341912613852</v>
       </c>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
@@ -3843,7 +3843,7 @@
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
@@ -3896,14 +3896,14 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Mt / capita</t>
+          <t>t/cap/year</t>
         </is>
       </c>
       <c r="K49" t="n">
         <v>2050</v>
       </c>
       <c r="L49" t="n">
-        <v>2.321482602218339e-07</v>
+        <v>0.2321482602218339</v>
       </c>
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>aus EUCalc-Tool (Life), Population aus Datensatz</t>
+          <t>calculated in EUCalc-Tool (Life Scenario), for details see script https://github.com/Sufficiency-Quantification/SufficiencyIndicators_EU-Calc/tree/main</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">

</xml_diff>

<commit_message>
Changed output for meat consumption to per day
</commit_message>
<xml_diff>
--- a/output/input_for_scenario_analysis.xlsx
+++ b/output/input_for_scenario_analysis.xlsx
@@ -1134,7 +1134,7 @@
         <v>2015</v>
       </c>
       <c r="L10" t="n">
-        <v>111399.140625</v>
+        <v>305.203125</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
@@ -1986,7 +1986,7 @@
         <v>2050</v>
       </c>
       <c r="L22" t="n">
-        <v>30712.0125</v>
+        <v>84.1425</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
@@ -2838,7 +2838,7 @@
         <v>2015</v>
       </c>
       <c r="L34" t="n">
-        <v>117681.5898114887</v>
+        <v>322.4153145520239</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
@@ -3690,7 +3690,7 @@
         <v>2050</v>
       </c>
       <c r="L46" t="n">
-        <v>30693.48093538231</v>
+        <v>84.09172859008852</v>
       </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>

</xml_diff>